<commit_message>
Added schematics for receipt and purchases tables
</commit_message>
<xml_diff>
--- a/Databases/DEMO database.xlsx
+++ b/Databases/DEMO database.xlsx
@@ -5,30 +5,38 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macie\Documents\Projects\Untilted_irl_trade_skill_master\Databases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macie\Documents\Projects\IRL_TSM\Databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DBFB271-E014-4C6F-A858-A191EDE07260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A939A369-AF0A-4327-ADB5-E01D4BA0028F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10030" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="specific_product" sheetId="1" r:id="rId1"/>
+    <sheet name="receipt" sheetId="2" r:id="rId2"/>
+    <sheet name="purchases" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
-  <si>
-    <t>ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
   <si>
     <t>NAME</t>
   </si>
@@ -118,6 +126,36 @@
   </si>
   <si>
     <t>Selenium [mcg] (REAL)</t>
+  </si>
+  <si>
+    <t>ID [barcode] (INT)</t>
+  </si>
+  <si>
+    <t>rowid</t>
+  </si>
+  <si>
+    <t>date (?)</t>
+  </si>
+  <si>
+    <t>receipt_image (BLOB)</t>
+  </si>
+  <si>
+    <t>shop (TEXT)</t>
+  </si>
+  <si>
+    <t>product_id (INT)</t>
+  </si>
+  <si>
+    <t>receipt_id (INT)</t>
+  </si>
+  <si>
+    <t>amount_bought (REAL)</t>
+  </si>
+  <si>
+    <t>unit (TEXT)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kg, g, l, ml, pc </t>
   </si>
 </sst>
 </file>
@@ -447,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -486,209 +524,307 @@
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" t="s">
+        <v>26</v>
+      </c>
+      <c r="V1" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>23</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AL1" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="O1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>17</v>
-      </c>
-      <c r="R1" t="s">
-        <v>18</v>
-      </c>
-      <c r="S1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X1" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>1</v>
+        <f>A2+1</f>
+        <v>2</v>
       </c>
       <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>2</v>
+        <f t="shared" ref="A4:A21" si="0">A3+1</f>
+        <v>3</v>
       </c>
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>6</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="D9" s="1"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>9</v>
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>10</v>
+        <f t="shared" si="0"/>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>12</v>
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>13</v>
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>14</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>15</v>
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>16</v>
+        <f t="shared" si="0"/>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>17</v>
+        <f t="shared" si="0"/>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>18</v>
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>19</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA5D5236-B24F-47AD-952E-2CAC64D9D220}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="18.90625" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9AD225D-7488-4DE1-A840-F114D6604DBA}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="14.453125" customWidth="1"/>
+    <col min="3" max="3" width="13.7265625" customWidth="1"/>
+    <col min="4" max="4" width="20.36328125" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new TABLE to schematic of the database
</commit_message>
<xml_diff>
--- a/Databases/DEMO database.xlsx
+++ b/Databases/DEMO database.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macie\Documents\Projects\IRL_TSM\Databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DDF49C-7EEF-4F3F-A1F4-422085754533}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A013944-F1FE-4C29-BCF0-7155406510A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10030" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10030" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" r:id="rId1"/>
-    <sheet name="receipts" sheetId="2" r:id="rId2"/>
-    <sheet name="purchases" sheetId="3" r:id="rId3"/>
+    <sheet name="nutrition_facts" sheetId="4" r:id="rId2"/>
+    <sheet name="receipts" sheetId="2" r:id="rId3"/>
+    <sheet name="purchases" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>NAME</t>
   </si>
@@ -485,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -553,69 +554,6 @@
       <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>17</v>
-      </c>
-      <c r="T1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>26</v>
-      </c>
-      <c r="V1" t="s">
-        <v>19</v>
-      </c>
-      <c r="W1" t="s">
-        <v>20</v>
-      </c>
-      <c r="X1" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>25</v>
-      </c>
       <c r="AL1" t="s">
         <v>11</v>
       </c>
@@ -754,6 +692,92 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38EA1072-DB47-4780-B724-1AD91AB8E00D}">
+  <dimension ref="A1:W1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>21</v>
+      </c>
+      <c r="R1" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA5D5236-B24F-47AD-952E-2CAC64D9D220}">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -787,7 +811,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9AD225D-7488-4DE1-A840-F114D6604DBA}">
   <dimension ref="A1:E2"/>
   <sheetViews>

</xml_diff>

<commit_message>
Giving up on the project (for a while at least)
</commit_message>
<xml_diff>
--- a/Databases/DEMO database.xlsx
+++ b/Databases/DEMO database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\macie\Documents\Projects\IRL_TSM\Databases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A013944-F1FE-4C29-BCF0-7155406510A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3844F3D4-B6A2-4B93-BFA7-190D33B0B7AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10030" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="products" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>NAME</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>date (TEXT)</t>
-  </si>
-  <si>
-    <t>image (BLOB)</t>
   </si>
 </sst>
 </file>
@@ -695,11 +692,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38EA1072-DB47-4780-B724-1AD91AB8E00D}">
   <dimension ref="A1:W1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="16.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -774,15 +771,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA5D5236-B24F-47AD-952E-2CAC64D9D220}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -792,7 +790,7 @@
     <col min="4" max="4" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>31</v>
       </c>
@@ -801,9 +799,6 @@
       </c>
       <c r="C1" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -815,7 +810,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9AD225D-7488-4DE1-A840-F114D6604DBA}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>

</xml_diff>